<commit_message>
HP Server Value is Update
</commit_message>
<xml_diff>
--- a/index_report_export.xlsx
+++ b/index_report_export.xlsx
@@ -463,13 +463,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="n">
-        <v>1132150</v>
+        <v>1071000</v>
       </c>
       <c r="D2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -482,10 +482,10 @@
         <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>1131600</v>
+        <v>1070650</v>
       </c>
       <c r="D3" t="n">
-        <v>-0</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="4">
@@ -495,13 +495,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" t="n">
-        <v>1131200</v>
+        <v>1071300</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5">
@@ -514,7 +514,7 @@
         <v>90</v>
       </c>
       <c r="C5" t="n">
-        <v>3394950</v>
+        <v>3212950</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -665,21 +665,21 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>DELL</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Inspiron 13 5310</t>
+          <t>probook 440 G8</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Masum Billah</t>
+          <t>Md. Tariqul Islam</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>i7</t>
+          <t>i5</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -703,10 +703,14 @@
       <c r="K2" t="n">
         <v>11</v>
       </c>
-      <c r="L2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2GB</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -715,20 +719,20 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>115000</v>
+        <v>85000</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="R2" t="n">
-        <v>69000</v>
+        <v>59500</v>
       </c>
     </row>
     <row r="3">
@@ -743,26 +747,26 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>HP Laptop</t>
+          <t>Dell Laptop</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>15s-Fq5317TU</t>
+          <t>Inspiron 15 3511</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Willam Pintu</t>
+          <t>Tareq</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>In Stock</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -779,12 +783,12 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -793,20 +797,20 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>72500</v>
+        <v>75000</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R3" t="n">
-        <v>50750</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="4">
@@ -821,26 +825,26 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>HP Laptop</t>
+          <t>DELL</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>RTL8822CE</t>
+          <t>Inspiron 3511</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Aminul T3</t>
+          <t>Safaur Rahman</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>In Stock</t>
+          <t>User</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -853,13 +857,17 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>500</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>12</v>
-      </c>
-      <c r="L4" t="inlineStr"/>
+        <v>11</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2GB</t>
+        </is>
+      </c>
       <c r="M4" t="inlineStr">
         <is>
           <t>Good</t>
@@ -871,7 +879,7 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>72500</v>
+        <v>75000</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -884,7 +892,7 @@
         </is>
       </c>
       <c r="R4" t="n">
-        <v>43500</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="5">
@@ -899,26 +907,26 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Dell Laptop</t>
+          <t>DELL</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Inspiron 5410</t>
+          <t>Inspiron 3493</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Salim</t>
+          <t>Mokles(FPT)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>In Stock</t>
+          <t>User</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -927,20 +935,24 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>11</v>
-      </c>
-      <c r="L5" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>128MB</t>
+        </is>
+      </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -953,16 +965,16 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>50%</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="R5" t="n">
-        <v>45000</v>
+        <v>37500</v>
       </c>
     </row>
     <row r="6">
@@ -977,7 +989,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -991,7 +1003,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Selim(FPT)</t>
+          <t>Sadman(FPT)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1018,7 +1030,7 @@
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -1031,16 +1043,16 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R6" t="n">
-        <v>24000</v>
+        <v>28800</v>
       </c>
     </row>
     <row r="7">
@@ -1055,7 +1067,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1064,12 +1076,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>830 G5</t>
+          <t>Elitbook 840 G3</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Ibrahim(FPT)</t>
+          <t>Md Nayem</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1083,11 +1095,11 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>256</t>
+          <t>500</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -1105,7 +1117,7 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>55000</v>
+        <v>48000</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
@@ -1118,7 +1130,7 @@
         </is>
       </c>
       <c r="R7" t="n">
-        <v>22000</v>
+        <v>19200</v>
       </c>
     </row>
     <row r="8">
@@ -1133,7 +1145,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1142,12 +1154,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Elitbook</t>
+          <t>HSN-112C</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Md. Gaznobi Liton</t>
+          <t>Rubel Biswas</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1171,14 +1183,10 @@
       <c r="K8" t="n">
         <v>8</v>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>128MB</t>
-        </is>
-      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1187,20 +1195,20 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>45000</v>
+        <v>50000</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>70%</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R8" t="n">
-        <v>18000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="9">
@@ -1297,7 +1305,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1311,7 +1319,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Touhidur Rahman (Abir)</t>
+          <t>Jahidul Islam</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1375,21 +1383,21 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>DELL</t>
+          <t>LENOVO</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>inspiron 3542</t>
+          <t>X230</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Tareq</t>
+          <t>Afjal hossain</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1399,7 +1407,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>i3</t>
+          <t>i5</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1407,11 +1415,11 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>256</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr">
@@ -1425,7 +1433,7 @@
         </is>
       </c>
       <c r="O11" t="n">
-        <v>32000</v>
+        <v>28000</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
@@ -1438,13 +1446,13 @@
         </is>
       </c>
       <c r="R11" t="n">
-        <v>6400</v>
+        <v>5600</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1453,76 +1461,76 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Dell Laptop</t>
+          <t>DELL</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>P106F</t>
+          <t>inspiron 3542</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Nahid</t>
+          <t>Tareq</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>In Stock</t>
+          <t>User</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>i7</t>
+          <t>i3</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="K12" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>reconditioned</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>110000</v>
+        <v>32000</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="R12" t="n">
-        <v>66000</v>
+        <v>6400</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1531,70 +1539,70 @@
         </is>
       </c>
       <c r="C13" t="n">
+        <v>33</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>HP</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>440-G2</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Hasan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>i3</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
         <v>4</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>HP Laptop</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>15s-fq5317TU</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Jahidul Kabir</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>i5</t>
-        </is>
-      </c>
-      <c r="I13" t="n">
-        <v>8</v>
-      </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="K13" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>reconditioned</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>72500</v>
+        <v>30000</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="R13" t="n">
-        <v>50750</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="14">
@@ -1609,31 +1617,31 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>DELL</t>
+          <t>Dell Laptop</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Inspiron 3511</t>
+          <t>P106F</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Safaur Rahman</t>
+          <t>Nahid</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>In Stock</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>i5</t>
+          <t>i7</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1647,11 +1655,7 @@
       <c r="K14" t="n">
         <v>11</v>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>2GB</t>
-        </is>
-      </c>
+      <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr">
         <is>
           <t>Good</t>
@@ -1663,7 +1667,7 @@
         </is>
       </c>
       <c r="O14" t="n">
-        <v>75000</v>
+        <v>110000</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
@@ -1676,7 +1680,7 @@
         </is>
       </c>
       <c r="R14" t="n">
-        <v>45000</v>
+        <v>66000</v>
       </c>
     </row>
     <row r="15">
@@ -1691,52 +1695,48 @@
         </is>
       </c>
       <c r="C15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>HP Laptop</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>15s-fq5317TU</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Jahidul Kabir</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>i5</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>8</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
         <v>12</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>DELL</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Inspiron 3493</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Mokles(FPT)</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>User</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>i5</t>
-        </is>
-      </c>
-      <c r="I15" t="n">
-        <v>4</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="K15" t="n">
-        <v>10</v>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>128MB</t>
-        </is>
-      </c>
+      <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -1745,20 +1745,20 @@
         </is>
       </c>
       <c r="O15" t="n">
-        <v>75000</v>
+        <v>72500</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="R15" t="n">
-        <v>37500</v>
+        <v>50750</v>
       </c>
     </row>
     <row r="16">
@@ -1773,21 +1773,21 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>LENOVO</t>
+          <t>DELL</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>V14-G2-ITL</t>
+          <t>Inspiron 3511</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Riday(FPT)</t>
+          <t>Md Mehrab</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1797,24 +1797,28 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>i3</t>
+          <t>i5</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>500</t>
         </is>
       </c>
       <c r="K16" t="n">
         <v>11</v>
       </c>
-      <c r="L16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2GB</t>
+        </is>
+      </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -1823,20 +1827,20 @@
         </is>
       </c>
       <c r="O16" t="n">
-        <v>48000</v>
+        <v>75000</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="R16" t="n">
-        <v>28800</v>
+        <v>52500</v>
       </c>
     </row>
     <row r="17">
@@ -1851,21 +1855,21 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>DELL</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>440-G4</t>
+          <t>Inspiron 3511</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Md Aminul Islam</t>
+          <t>Ashraful Ul Anam</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1875,7 +1879,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>i7</t>
+          <t>i5</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1883,11 +1887,11 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>500</t>
         </is>
       </c>
       <c r="K17" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
@@ -1896,29 +1900,29 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>reconditioned</t>
+          <t>new</t>
         </is>
       </c>
       <c r="O17" t="n">
-        <v>60000</v>
+        <v>75000</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R17" t="n">
-        <v>24000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="18">
@@ -1933,7 +1937,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1942,12 +1946,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Elitbook 840 G3</t>
+          <t>15s-fq2643TU</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Md Nayem</t>
+          <t>Abu Sayed</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1961,7 +1965,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1969,34 +1973,34 @@
         </is>
       </c>
       <c r="K18" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>reconditioned</t>
+          <t>new</t>
         </is>
       </c>
       <c r="O18" t="n">
-        <v>48000</v>
+        <v>70000</v>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>50%</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="R18" t="n">
-        <v>19200</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="19">
@@ -2011,17 +2015,21 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>HP Laptop</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
+          <t>DELL</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Inspiron 3511</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Rasel (FADS)</t>
+          <t>Suruj Office</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -2031,7 +2039,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>i5</t>
+          <t>i3</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -2039,15 +2047,13 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>256</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>128MB</t>
-        </is>
-      </c>
+          <t>128/256</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>11</v>
+      </c>
+      <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr">
         <is>
           <t>Good</t>
@@ -2055,15 +2061,15 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>reconditioned</t>
+          <t>new</t>
         </is>
       </c>
       <c r="O19" t="n">
-        <v>45000</v>
+        <v>50000</v>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>70%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
@@ -2072,7 +2078,7 @@
         </is>
       </c>
       <c r="R19" t="n">
-        <v>13500</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="20">
@@ -2087,7 +2093,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -2096,12 +2102,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>X230</t>
+          <t>V14-G2-ITL</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Jahidul Islam</t>
+          <t>Riday(FPT)</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -2111,7 +2117,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>i5</t>
+          <t>i3</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2119,38 +2125,38 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>256</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="K20" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>reconditioned</t>
+          <t>new</t>
         </is>
       </c>
       <c r="O20" t="n">
-        <v>28000</v>
+        <v>48000</v>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R20" t="n">
-        <v>5600</v>
+        <v>28800</v>
       </c>
     </row>
     <row r="21">
@@ -2165,21 +2171,21 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>LENOVO</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>X230</t>
+          <t>440-G4</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Afjal hossain</t>
+          <t>Md Aminul Islam</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -2189,24 +2195,28 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>i5</t>
+          <t>i7</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>256</t>
+          <t>240</t>
         </is>
       </c>
       <c r="K21" t="n">
-        <v>3</v>
-      </c>
-      <c r="L21" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>2GB</t>
+        </is>
+      </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2215,20 +2225,20 @@
         </is>
       </c>
       <c r="O21" t="n">
-        <v>28000</v>
+        <v>60000</v>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>60%</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="R21" t="n">
-        <v>5600</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="22">
@@ -2243,21 +2253,21 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>DELL</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Latitute 3350</t>
+          <t>Probook 440 G4</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Debasish Mondol</t>
+          <t>Faysal Hossain(Design)</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -2267,25 +2277,21 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>i3</t>
+          <t>i7</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>128/1000</t>
         </is>
       </c>
       <c r="K22" t="n">
-        <v>5</v>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>128MB</t>
-        </is>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr">
         <is>
           <t>Moderate</t>
@@ -2297,7 +2303,7 @@
         </is>
       </c>
       <c r="O22" t="n">
-        <v>35000</v>
+        <v>95000</v>
       </c>
       <c r="P22" t="inlineStr">
         <is>
@@ -2310,13 +2316,13 @@
         </is>
       </c>
       <c r="R22" t="n">
-        <v>7000</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2325,7 +2331,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -2334,12 +2340,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>probook 440 G8</t>
+          <t>830 G5</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Md. Tariqul Islam</t>
+          <t>Ibrahim(FPT)</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2353,21 +2359,17 @@
         </is>
       </c>
       <c r="I23" t="n">
+        <v>4</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>256</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
         <v>8</v>
       </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
-      </c>
-      <c r="K23" t="n">
-        <v>11</v>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>2GB</t>
-        </is>
-      </c>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr">
         <is>
           <t>Excellent</t>
@@ -2375,15 +2377,15 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>reconditioned</t>
         </is>
       </c>
       <c r="O23" t="n">
-        <v>85000</v>
+        <v>55000</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>60%</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
@@ -2392,13 +2394,13 @@
         </is>
       </c>
       <c r="R23" t="n">
-        <v>59500</v>
+        <v>22000</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2407,21 +2409,21 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>DELL</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Inspiron 3511</t>
+          <t>Elitbook840 G3</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Md Mehrab</t>
+          <t>Suruj</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2439,48 +2441,44 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>240</t>
         </is>
       </c>
       <c r="K24" t="n">
-        <v>11</v>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>2GB</t>
-        </is>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>reconditioned</t>
         </is>
       </c>
       <c r="O24" t="n">
-        <v>75000</v>
+        <v>45000</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>70%</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R24" t="n">
-        <v>52500</v>
+        <v>13500</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2489,26 +2487,26 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Dell Laptop</t>
+          <t>Lenovo Thinkpad</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Inspiron 15 3511</t>
+          <t>X230</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Tareq</t>
+          <t>Biplob Hossen</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>In Stock</t>
+          <t>User</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2517,48 +2515,48 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>256</t>
         </is>
       </c>
       <c r="K25" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>reconditioned</t>
         </is>
       </c>
       <c r="O25" t="n">
-        <v>75000</v>
+        <v>28000</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="R25" t="n">
-        <v>45000</v>
+        <v>5600</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2567,74 +2565,66 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>DELL</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Inspiron 3511</t>
-        </is>
-      </c>
+          <t>ASUS</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Ashraful Ul Anam</t>
+          <t>Ashraful</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>In Stock</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>i5</t>
+          <t>i3</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="K26" t="n">
-        <v>11</v>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>2GB</t>
-        </is>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>reconditioned</t>
         </is>
       </c>
       <c r="O26" t="n">
-        <v>75000</v>
+        <v>28000</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="R26" t="n">
-        <v>45000</v>
+        <v>5600</v>
       </c>
     </row>
     <row r="27">
@@ -2649,21 +2639,21 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>DELL</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>15s-fq2643TU</t>
+          <t>Inspiron 13 5310</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Abu Sayed</t>
+          <t>Masum Billah</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2673,7 +2663,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>i5</t>
+          <t>i7</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2690,7 +2680,7 @@
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -2699,20 +2689,20 @@
         </is>
       </c>
       <c r="O27" t="n">
-        <v>70000</v>
+        <v>115000</v>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R27" t="n">
-        <v>35000</v>
+        <v>69000</v>
       </c>
     </row>
     <row r="28">
@@ -2727,48 +2717,48 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>DELL</t>
+          <t>HP Laptop</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Inspiron 3511</t>
+          <t>15s-Fq5317TU</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Suruj Office</t>
+          <t>Willam Pintu</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>In Stock</t>
+          <t>User</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>i3</t>
+          <t>i5</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>128/256</t>
+          <t>500</t>
         </is>
       </c>
       <c r="K28" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -2777,20 +2767,20 @@
         </is>
       </c>
       <c r="O28" t="n">
-        <v>50000</v>
+        <v>72500</v>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="R28" t="n">
-        <v>30000</v>
+        <v>50750</v>
       </c>
     </row>
     <row r="29">
@@ -2805,43 +2795,43 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>LENOVO</t>
+          <t>HP Laptop</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>V14-G2-ITL</t>
+          <t>RTL8822CE</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Sadman(FPT)</t>
+          <t>Aminul T3</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>In Stock</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>i3</t>
+          <t>i5</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>240</t>
         </is>
       </c>
       <c r="K29" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr">
@@ -2855,7 +2845,7 @@
         </is>
       </c>
       <c r="O29" t="n">
-        <v>48000</v>
+        <v>72500</v>
       </c>
       <c r="P29" t="inlineStr">
         <is>
@@ -2868,7 +2858,7 @@
         </is>
       </c>
       <c r="R29" t="n">
-        <v>28800</v>
+        <v>43500</v>
       </c>
     </row>
     <row r="30">
@@ -2883,31 +2873,31 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Dell Laptop</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Probook 440 G4</t>
+          <t>Inspiron 5410</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Faysal Hossain(Design)</t>
+          <t>Salim</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>In Stock</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>i7</t>
+          <t>i5</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2915,38 +2905,38 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>128/1000</t>
+          <t>500</t>
         </is>
       </c>
       <c r="K30" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>reconditioned</t>
+          <t>new</t>
         </is>
       </c>
       <c r="O30" t="n">
-        <v>95000</v>
+        <v>75000</v>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R30" t="n">
-        <v>19000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="31">
@@ -2961,21 +2951,21 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>LENOVO</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Elitbook840 G3</t>
+          <t>V14-G2-ITL</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Suruj</t>
+          <t>Selim(FPT)</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2985,46 +2975,46 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>i5</t>
+          <t>i3</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="K31" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>reconditioned</t>
+          <t>new</t>
         </is>
       </c>
       <c r="O31" t="n">
-        <v>45000</v>
+        <v>48000</v>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>70%</t>
+          <t>50%</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="R31" t="n">
-        <v>13500</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="32">
@@ -3039,7 +3029,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -3048,12 +3038,12 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>HSN-112C</t>
+          <t>Elitbook</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Rubel Biswas</t>
+          <t>Md. Gaznobi Liton</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -3077,10 +3067,14 @@
       <c r="K32" t="n">
         <v>8</v>
       </c>
-      <c r="L32" t="inlineStr"/>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>128MB</t>
+        </is>
+      </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
@@ -3089,20 +3083,20 @@
         </is>
       </c>
       <c r="O32" t="n">
-        <v>50000</v>
+        <v>45000</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>70%</t>
+          <t>60%</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>15000</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="33">
@@ -3117,26 +3111,22 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Lenovo Thinkpad</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>X230</t>
-        </is>
-      </c>
+          <t>HP Laptop</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Biplob Hossen</t>
+          <t>Rasel (FADS)</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>In Stock</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -3152,13 +3142,15 @@
           <t>256</t>
         </is>
       </c>
-      <c r="K33" t="n">
-        <v>3</v>
-      </c>
-      <c r="L33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>128MB</t>
+        </is>
+      </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
@@ -3167,20 +3159,20 @@
         </is>
       </c>
       <c r="O33" t="n">
-        <v>28000</v>
+        <v>45000</v>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>70%</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R33" t="n">
-        <v>5600</v>
+        <v>13500</v>
       </c>
     </row>
     <row r="34">
@@ -3195,21 +3187,21 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>LENOVO</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>440-G2</t>
+          <t>X230</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Hasan</t>
+          <t>Touhidur Rahman (Abir)</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -3219,7 +3211,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>i3</t>
+          <t>i5</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -3227,11 +3219,11 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>256</t>
         </is>
       </c>
       <c r="K34" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr">
@@ -3245,7 +3237,7 @@
         </is>
       </c>
       <c r="O34" t="n">
-        <v>30000</v>
+        <v>28000</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
@@ -3258,7 +3250,7 @@
         </is>
       </c>
       <c r="R34" t="n">
-        <v>6000</v>
+        <v>5600</v>
       </c>
     </row>
     <row r="35">
@@ -3273,22 +3265,26 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>ASUS</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr"/>
+          <t>DELL</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Latitute 3350</t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Ashraful</t>
+          <t>Debasish Mondol</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>In Stock</t>
+          <t>User</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -3301,13 +3297,17 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>500</t>
         </is>
       </c>
       <c r="K35" t="n">
-        <v>6</v>
-      </c>
-      <c r="L35" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>128MB</t>
+        </is>
+      </c>
       <c r="M35" t="inlineStr">
         <is>
           <t>Moderate</t>
@@ -3319,7 +3319,7 @@
         </is>
       </c>
       <c r="O35" t="n">
-        <v>28000</v>
+        <v>35000</v>
       </c>
       <c r="P35" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         </is>
       </c>
       <c r="R35" t="n">
-        <v>5600</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="36">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>650000</v>
+        <v>390000</v>
       </c>
       <c r="P36" t="inlineStr">
         <is>
@@ -3406,7 +3406,7 @@
         </is>
       </c>
       <c r="R36" t="n">
-        <v>455000</v>
+        <v>273000</v>
       </c>
     </row>
     <row r="37">
@@ -3421,7 +3421,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -3435,52 +3435,56 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Mostak</t>
+          <t>Nayon Design</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>3rd Floor</t>
+          <t>2nd Floor</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>i3</t>
+          <t>i9</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>128/1000</t>
+          <t>256/1000</t>
         </is>
       </c>
       <c r="K37" t="n">
-        <v>10</v>
-      </c>
-      <c r="L37" t="inlineStr"/>
+        <v>13</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>4GB</t>
+        </is>
+      </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>55000</v>
+        <v>280000</v>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="R37" t="n">
-        <v>33000</v>
+        <v>196000</v>
       </c>
     </row>
     <row r="38">
@@ -3495,7 +3499,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -3504,12 +3508,12 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>HP ProDesk</t>
+          <t>Clone PC</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Server Room</t>
+          <t>Kawser</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -3519,7 +3523,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>i5</t>
+          <t>i3</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3527,40 +3531,40 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>256/1000</t>
         </is>
       </c>
       <c r="K38" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="n">
-        <v>75000</v>
+        <v>55000</v>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R38" t="n">
-        <v>7500</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3569,7 +3573,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -3583,62 +3587,58 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Humayon Design</t>
+          <t>Comercial Room</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>3rd Floor</t>
+          <t>2nd Floor</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>i9</t>
+          <t>i3</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>256/1000</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="K39" t="n">
-        <v>13</v>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>4GB</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="n">
-        <v>280000</v>
+        <v>35000</v>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>50%</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="R39" t="n">
-        <v>196000</v>
+        <v>17500</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3647,7 +3647,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -3656,12 +3656,12 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Clone PC</t>
+          <t>HP ProDesk</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Design Team</t>
+          <t>Server Room</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -3671,46 +3671,42 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>i9</t>
+          <t>i5</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>256/1000</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="K40" t="n">
-        <v>13</v>
-      </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>4GB</t>
-        </is>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="N40" t="inlineStr"/>
       <c r="O40" t="n">
-        <v>280000</v>
+        <v>75000</v>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="R40" t="n">
-        <v>196000</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="41">
@@ -3725,7 +3721,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -3739,12 +3735,12 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Nayon Design</t>
+          <t>Humayon Design</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2nd Floor</t>
+          <t>3rd Floor</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3803,7 +3799,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -3817,7 +3813,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Kawser</t>
+          <t>Design Team</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -3827,11 +3823,11 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>i3</t>
+          <t>i9</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3839,30 +3835,34 @@
         </is>
       </c>
       <c r="K42" t="n">
-        <v>10</v>
-      </c>
-      <c r="L42" t="inlineStr"/>
+        <v>13</v>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>4GB</t>
+        </is>
+      </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="n">
-        <v>55000</v>
+        <v>280000</v>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="R42" t="n">
-        <v>33000</v>
+        <v>196000</v>
       </c>
     </row>
     <row r="43">
@@ -3877,66 +3877,66 @@
         </is>
       </c>
       <c r="C43" t="n">
+        <v>10</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Desktop</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Clone PC</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>IT Room</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2nd Floor</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>i9</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>32</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>1000/2000</t>
+        </is>
+      </c>
+      <c r="K43" t="n">
         <v>11</v>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Desktop</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Clone PC</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Faysal Comercial</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>2nd Floor</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>i5</t>
-        </is>
-      </c>
-      <c r="I43" t="n">
-        <v>8</v>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="K43" t="n">
-        <v>10</v>
       </c>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="n">
-        <v>85000</v>
+        <v>220000</v>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="R43" t="n">
-        <v>8500</v>
+        <v>154000</v>
       </c>
     </row>
     <row r="44">
@@ -3951,7 +3951,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -3965,7 +3965,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Comercial Room</t>
+          <t>Faysal Comercial</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -3975,11 +3975,11 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>i3</t>
+          <t>i5</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -3987,30 +3987,30 @@
         </is>
       </c>
       <c r="K44" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="n">
-        <v>35000</v>
+        <v>85000</v>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R44" t="n">
-        <v>17500</v>
+        <v>8500</v>
       </c>
     </row>
     <row r="45">
@@ -4329,66 +4329,66 @@
         </is>
       </c>
       <c r="C49" t="n">
+        <v>8</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Desktop</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Clone PC</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Mostak</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>3rd Floor</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>i3</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>8</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>128/1000</t>
+        </is>
+      </c>
+      <c r="K49" t="n">
         <v>10</v>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Desktop</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>Clone PC</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>IT Room</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>2nd Floor</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>i9</t>
-        </is>
-      </c>
-      <c r="I49" t="n">
-        <v>32</v>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>1000/2000</t>
-        </is>
-      </c>
-      <c r="K49" t="n">
-        <v>11</v>
       </c>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="n">
-        <v>220000</v>
+        <v>55000</v>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R49" t="n">
-        <v>154000</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="50">
@@ -4613,7 +4613,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -4627,7 +4627,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>IT Room</t>
+          <t>Nayon</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -4675,26 +4675,26 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>HP Monitor</t>
+          <t>ASUS Monitor</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>M22f</t>
+          <t>VP229HE</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Enamul</t>
+          <t>Faysal Comercial</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>3rd Floor</t>
+          <t>2nd Floor</t>
         </is>
       </c>
       <c r="H54" t="inlineStr"/>
@@ -4737,16 +4737,16 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>HP Monitor</t>
+          <t>Dell Monitor</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>LV1911</t>
+          <t>52240Lc</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4771,7 +4771,7 @@
       </c>
       <c r="N55" t="inlineStr"/>
       <c r="O55" t="n">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="P55" t="inlineStr">
         <is>
@@ -4784,7 +4784,7 @@
         </is>
       </c>
       <c r="R55" t="n">
-        <v>7000</v>
+        <v>8400</v>
       </c>
     </row>
     <row r="56">
@@ -4799,26 +4799,26 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>SAMSUNG</t>
+          <t>Dell Monitor</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>S19C300B</t>
+          <t>G2QR5D2</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Common PC</t>
+          <t>Kawser</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>3th Floor</t>
+          <t>3rd Floor</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
@@ -4828,25 +4828,25 @@
       <c r="L56" t="inlineStr"/>
       <c r="M56" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="N56" t="inlineStr"/>
       <c r="O56" t="n">
-        <v>9500</v>
+        <v>11000</v>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="R56" t="n">
-        <v>5700</v>
+        <v>7700</v>
       </c>
     </row>
     <row r="57">
@@ -4985,7 +4985,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -5047,21 +5047,21 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Dell Monitor</t>
+          <t>HP Monitor</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>G2QR5D2</t>
+          <t>LV1911</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Kawser</t>
+          <t>Design Team</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -5081,7 +5081,7 @@
       </c>
       <c r="N60" t="inlineStr"/>
       <c r="O60" t="n">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="P60" t="inlineStr">
         <is>
@@ -5094,13 +5094,13 @@
         </is>
       </c>
       <c r="R60" t="n">
-        <v>7700</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5109,26 +5109,26 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>HP Monitor</t>
+          <t>SAMSUNG</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>M22f</t>
+          <t>S19C300B</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Nayon</t>
+          <t>Common PC</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2nd Floor</t>
+          <t>3th Floor</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
@@ -5138,25 +5138,25 @@
       <c r="L61" t="inlineStr"/>
       <c r="M61" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="n">
-        <v>15500</v>
+        <v>9500</v>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="R61" t="n">
-        <v>10850</v>
+        <v>5700</v>
       </c>
     </row>
     <row r="62">
@@ -5171,21 +5171,21 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>ASUS Monitor</t>
+          <t>HP Monitor</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>VP229HE</t>
+          <t>M22f</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Faysal Comercial</t>
+          <t>IT Room</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -5233,21 +5233,21 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Dell Monitor</t>
+          <t>HP Monitor</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>52240Lc</t>
+          <t>M22f</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Design Team</t>
+          <t>Enamul</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -5267,7 +5267,7 @@
       </c>
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="n">
-        <v>12000</v>
+        <v>15500</v>
       </c>
       <c r="P63" t="inlineStr">
         <is>
@@ -5280,7 +5280,7 @@
         </is>
       </c>
       <c r="R63" t="n">
-        <v>8400</v>
+        <v>10850</v>
       </c>
     </row>
     <row r="64">
@@ -5419,22 +5419,22 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>EPSON</t>
+          <t>EPSON A3</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>L3250</t>
+          <t>C722B1</t>
         </is>
       </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>3rd Floor CO Sir Room</t>
+          <t>2nd Floor Marketing Room</t>
         </is>
       </c>
       <c r="H66" t="inlineStr"/>
@@ -5449,7 +5449,7 @@
       </c>
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="n">
-        <v>21000</v>
+        <v>80000</v>
       </c>
       <c r="P66" t="inlineStr">
         <is>
@@ -5462,7 +5462,7 @@
         </is>
       </c>
       <c r="R66" t="n">
-        <v>14700</v>
+        <v>56000</v>
       </c>
     </row>
     <row r="67">
@@ -5477,7 +5477,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -5486,13 +5486,13 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Laser jet Pro M404dw</t>
+          <t>HP Laser Pro MFP M26nw</t>
         </is>
       </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2nd Floor Marketing Room</t>
+          <t>2nd Floor Director  Room</t>
         </is>
       </c>
       <c r="H67" t="inlineStr"/>
@@ -5507,7 +5507,7 @@
       </c>
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="n">
-        <v>42000</v>
+        <v>32000</v>
       </c>
       <c r="P67" t="inlineStr">
         <is>
@@ -5520,7 +5520,7 @@
         </is>
       </c>
       <c r="R67" t="n">
-        <v>29400</v>
+        <v>22400</v>
       </c>
     </row>
     <row r="68">
@@ -5535,22 +5535,22 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>T3 Project Printer</t>
+          <t>PANTUiM</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Canon F166400</t>
+          <t>P3010DW</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>GTL Warehouse</t>
+          <t>3rd Floor Supply Manager Room</t>
         </is>
       </c>
       <c r="H68" t="inlineStr"/>
@@ -5565,7 +5565,7 @@
       </c>
       <c r="N68" t="inlineStr"/>
       <c r="O68" t="n">
-        <v>15000</v>
+        <v>14000</v>
       </c>
       <c r="P68" t="inlineStr">
         <is>
@@ -5578,13 +5578,13 @@
         </is>
       </c>
       <c r="R68" t="n">
-        <v>10500</v>
+        <v>9800</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5593,22 +5593,22 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>EPSON A3</t>
+          <t>Canon</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>C722B1</t>
+          <t>F166500</t>
         </is>
       </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr">
         <is>
-          <t>2nd Floor Marketing Room</t>
+          <t>3rd Floor Accounts Room</t>
         </is>
       </c>
       <c r="H69" t="inlineStr"/>
@@ -5623,7 +5623,7 @@
       </c>
       <c r="N69" t="inlineStr"/>
       <c r="O69" t="n">
-        <v>80000</v>
+        <v>16000</v>
       </c>
       <c r="P69" t="inlineStr">
         <is>
@@ -5636,7 +5636,7 @@
         </is>
       </c>
       <c r="R69" t="n">
-        <v>56000</v>
+        <v>11200</v>
       </c>
     </row>
     <row r="70">
@@ -5651,22 +5651,22 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>EPSON</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>HP Laser Pro MFP M26nw</t>
+          <t>L3250</t>
         </is>
       </c>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2nd Floor Director  Room</t>
+          <t>3rd Floor CO Sir Room</t>
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
@@ -5681,7 +5681,7 @@
       </c>
       <c r="N70" t="inlineStr"/>
       <c r="O70" t="n">
-        <v>32000</v>
+        <v>21000</v>
       </c>
       <c r="P70" t="inlineStr">
         <is>
@@ -5694,7 +5694,7 @@
         </is>
       </c>
       <c r="R70" t="n">
-        <v>22400</v>
+        <v>14700</v>
       </c>
     </row>
     <row r="71">
@@ -5709,22 +5709,22 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Canon(Scaneer)</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Laser jet Pro M402dn</t>
+          <t>Canon EUROPA</t>
         </is>
       </c>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr">
         <is>
-          <t>3rd Floor  Open Space</t>
+          <t>2nd Floor Commercial  Room</t>
         </is>
       </c>
       <c r="H71" t="inlineStr"/>
@@ -5739,7 +5739,7 @@
       </c>
       <c r="N71" t="inlineStr"/>
       <c r="O71" t="n">
-        <v>22000</v>
+        <v>10000</v>
       </c>
       <c r="P71" t="inlineStr">
         <is>
@@ -5752,13 +5752,13 @@
         </is>
       </c>
       <c r="R71" t="n">
-        <v>15400</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5767,22 +5767,22 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Canon</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>F166500</t>
+          <t>Laser jet Pro M404dw</t>
         </is>
       </c>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr">
         <is>
-          <t>3rd Floor Accounts Room</t>
+          <t>2nd Floor Marketing Room</t>
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
@@ -5797,7 +5797,7 @@
       </c>
       <c r="N72" t="inlineStr"/>
       <c r="O72" t="n">
-        <v>16000</v>
+        <v>42000</v>
       </c>
       <c r="P72" t="inlineStr">
         <is>
@@ -5810,13 +5810,13 @@
         </is>
       </c>
       <c r="R72" t="n">
-        <v>11200</v>
+        <v>29400</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -5825,22 +5825,22 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>SAMSUNG</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Xpress M2820ND</t>
+          <t>Laser jet Pro M402dn</t>
         </is>
       </c>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr">
         <is>
-          <t>2nd Floor Commercial  Room</t>
+          <t>3rd Floor  Open Space</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
@@ -5855,7 +5855,7 @@
       </c>
       <c r="N73" t="inlineStr"/>
       <c r="O73" t="n">
-        <v>18000</v>
+        <v>22000</v>
       </c>
       <c r="P73" t="inlineStr">
         <is>
@@ -5868,13 +5868,13 @@
         </is>
       </c>
       <c r="R73" t="n">
-        <v>12600</v>
+        <v>15400</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5883,22 +5883,22 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Canon(Scaneer)</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Canon EUROPA</t>
+          <t>HP Laser 107w</t>
         </is>
       </c>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2nd Floor Commercial  Room</t>
+          <t>2nd Floor FPT Room</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
@@ -5913,7 +5913,7 @@
       </c>
       <c r="N74" t="inlineStr"/>
       <c r="O74" t="n">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="P74" t="inlineStr">
         <is>
@@ -5926,7 +5926,7 @@
         </is>
       </c>
       <c r="R74" t="n">
-        <v>7000</v>
+        <v>7700</v>
       </c>
     </row>
     <row r="75">
@@ -5941,22 +5941,22 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>PANTUiM</t>
+          <t>SAMSUNG</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>P3010DW</t>
+          <t>Xpress M2820ND</t>
         </is>
       </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr">
         <is>
-          <t>3rd Floor Supply Manager Room</t>
+          <t>2nd Floor Commercial  Room</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
@@ -5971,7 +5971,7 @@
       </c>
       <c r="N75" t="inlineStr"/>
       <c r="O75" t="n">
-        <v>14000</v>
+        <v>18000</v>
       </c>
       <c r="P75" t="inlineStr">
         <is>
@@ -5984,7 +5984,7 @@
         </is>
       </c>
       <c r="R75" t="n">
-        <v>9800</v>
+        <v>12600</v>
       </c>
     </row>
     <row r="76">
@@ -5999,22 +5999,22 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>T3 Project Printer</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>HP Laser 107w</t>
+          <t>Canon F166400</t>
         </is>
       </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr">
         <is>
-          <t>2nd Floor FPT Room</t>
+          <t>GTL Warehouse</t>
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
@@ -6029,7 +6029,7 @@
       </c>
       <c r="N76" t="inlineStr"/>
       <c r="O76" t="n">
-        <v>11000</v>
+        <v>15000</v>
       </c>
       <c r="P76" t="inlineStr">
         <is>
@@ -6042,7 +6042,7 @@
         </is>
       </c>
       <c r="R76" t="n">
-        <v>7700</v>
+        <v>10500</v>
       </c>
     </row>
     <row r="77">
@@ -6115,16 +6115,16 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>MikroTik Router Board</t>
+          <t>TP-Link Switch 24 Port</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>RB2011UiAS-RM</t>
+          <t>TL-SG1024D</t>
         </is>
       </c>
       <c r="F78" t="inlineStr"/>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="N78" t="inlineStr"/>
       <c r="O78" t="n">
-        <v>13000</v>
+        <v>7500</v>
       </c>
       <c r="P78" t="inlineStr">
         <is>
@@ -6154,7 +6154,7 @@
         </is>
       </c>
       <c r="R78" t="n">
-        <v>9100</v>
+        <v>5250</v>
       </c>
     </row>
     <row r="79">
@@ -6169,16 +6169,16 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Mikrotik Switch 16 Port</t>
+          <t>Cisco Switch 24 Port</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>CCR2004-16G-2S+</t>
+          <t>CBS350-24T-4G</t>
         </is>
       </c>
       <c r="F79" t="inlineStr"/>
@@ -6195,7 +6195,7 @@
       </c>
       <c r="N79" t="inlineStr"/>
       <c r="O79" t="n">
-        <v>85000</v>
+        <v>33000</v>
       </c>
       <c r="P79" t="inlineStr">
         <is>
@@ -6208,7 +6208,7 @@
         </is>
       </c>
       <c r="R79" t="n">
-        <v>59500</v>
+        <v>23100</v>
       </c>
     </row>
     <row r="80">
@@ -6223,16 +6223,16 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Cisco Switch 24 Port</t>
+          <t>UPS</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>CBS350-24T-4G</t>
+          <t>APC/SRCE6KUX1</t>
         </is>
       </c>
       <c r="F80" t="inlineStr"/>
@@ -6249,7 +6249,7 @@
       </c>
       <c r="N80" t="inlineStr"/>
       <c r="O80" t="n">
-        <v>33000</v>
+        <v>115000</v>
       </c>
       <c r="P80" t="inlineStr">
         <is>
@@ -6262,13 +6262,13 @@
         </is>
       </c>
       <c r="R80" t="n">
-        <v>23100</v>
+        <v>80500</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6277,16 +6277,16 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>KVM Switch 8 Port</t>
+          <t>ACS Soyal Conveter</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>KVM-0831</t>
+          <t>AR-727CM-V3</t>
         </is>
       </c>
       <c r="F81" t="inlineStr"/>
@@ -6303,7 +6303,7 @@
       </c>
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="n">
-        <v>8000</v>
+        <v>15000</v>
       </c>
       <c r="P81" t="inlineStr">
         <is>
@@ -6316,13 +6316,13 @@
         </is>
       </c>
       <c r="R81" t="n">
-        <v>5600</v>
+        <v>10500</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6331,16 +6331,16 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Hikvision DVR 8 Port</t>
+          <t>TP-Link Switch 8 Port</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>DS-720BHGH1-F2</t>
+          <t>T1500G-10PS</t>
         </is>
       </c>
       <c r="F82" t="inlineStr"/>
@@ -6357,7 +6357,7 @@
       </c>
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="n">
-        <v>12000</v>
+        <v>18000</v>
       </c>
       <c r="P82" t="inlineStr">
         <is>
@@ -6370,13 +6370,13 @@
         </is>
       </c>
       <c r="R82" t="n">
-        <v>8400</v>
+        <v>12600</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -6385,16 +6385,16 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Patch Panel 24 Port</t>
+          <t>Hikvision DVR 8 Port</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Net Key</t>
+          <t>DS-720BHGH1-F2</t>
         </is>
       </c>
       <c r="F83" t="inlineStr"/>
@@ -6411,7 +6411,7 @@
       </c>
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="n">
-        <v>3500</v>
+        <v>12000</v>
       </c>
       <c r="P83" t="inlineStr">
         <is>
@@ -6424,13 +6424,13 @@
         </is>
       </c>
       <c r="R83" t="n">
-        <v>2450</v>
+        <v>8400</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6484,7 +6484,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -6538,7 +6538,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -6547,14 +6547,18 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>UPS Battery 16 PCS</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr"/>
+          <t>MikroTik Router Board</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>RB2011UiAS-RM</t>
+        </is>
+      </c>
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="inlineStr"/>
@@ -6569,7 +6573,7 @@
       </c>
       <c r="N86" t="inlineStr"/>
       <c r="O86" t="n">
-        <v>160000</v>
+        <v>13000</v>
       </c>
       <c r="P86" t="inlineStr">
         <is>
@@ -6582,13 +6586,13 @@
         </is>
       </c>
       <c r="R86" t="n">
-        <v>112000</v>
+        <v>9100</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -6597,16 +6601,16 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>ACS Soyal Conveter</t>
+          <t>Mikrotik Switch 16 Port</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>AR-727CM-V3</t>
+          <t>CCR2004-16G-2S+</t>
         </is>
       </c>
       <c r="F87" t="inlineStr"/>
@@ -6623,7 +6627,7 @@
       </c>
       <c r="N87" t="inlineStr"/>
       <c r="O87" t="n">
-        <v>15000</v>
+        <v>85000</v>
       </c>
       <c r="P87" t="inlineStr">
         <is>
@@ -6636,13 +6640,13 @@
         </is>
       </c>
       <c r="R87" t="n">
-        <v>10500</v>
+        <v>59500</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -6651,16 +6655,16 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>TP-Link Switch 24 Port</t>
+          <t>KVM Switch 8 Port</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>TL-SG1024D</t>
+          <t>KVM-0831</t>
         </is>
       </c>
       <c r="F88" t="inlineStr"/>
@@ -6677,7 +6681,7 @@
       </c>
       <c r="N88" t="inlineStr"/>
       <c r="O88" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="P88" t="inlineStr">
         <is>
@@ -6690,7 +6694,7 @@
         </is>
       </c>
       <c r="R88" t="n">
-        <v>5250</v>
+        <v>5600</v>
       </c>
     </row>
     <row r="89">
@@ -6705,16 +6709,16 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>TP-Link Switch 8 Port</t>
+          <t>Hikvision DVR 16 Port</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>T1500G-10PS</t>
+          <t>DS-7216HQH1-K2</t>
         </is>
       </c>
       <c r="F89" t="inlineStr"/>
@@ -6731,7 +6735,7 @@
       </c>
       <c r="N89" t="inlineStr"/>
       <c r="O89" t="n">
-        <v>18000</v>
+        <v>23000</v>
       </c>
       <c r="P89" t="inlineStr">
         <is>
@@ -6744,7 +6748,7 @@
         </is>
       </c>
       <c r="R89" t="n">
-        <v>12600</v>
+        <v>16100</v>
       </c>
     </row>
     <row r="90">
@@ -6759,16 +6763,16 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Hikvision DVR 16 Port</t>
+          <t>Patch Panel 24 Port</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>DS-7216HQH1-K2</t>
+          <t>Net Key</t>
         </is>
       </c>
       <c r="F90" t="inlineStr"/>
@@ -6785,7 +6789,7 @@
       </c>
       <c r="N90" t="inlineStr"/>
       <c r="O90" t="n">
-        <v>23000</v>
+        <v>3500</v>
       </c>
       <c r="P90" t="inlineStr">
         <is>
@@ -6798,7 +6802,7 @@
         </is>
       </c>
       <c r="R90" t="n">
-        <v>16100</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="91">
@@ -6813,18 +6817,14 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>UPS</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>APC/SRCE6KUX1</t>
-        </is>
-      </c>
+          <t>UPS Battery 16 PCS</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="inlineStr"/>
@@ -6839,7 +6839,7 @@
       </c>
       <c r="N91" t="inlineStr"/>
       <c r="O91" t="n">
-        <v>115000</v>
+        <v>160000</v>
       </c>
       <c r="P91" t="inlineStr">
         <is>
@@ -6852,7 +6852,7 @@
         </is>
       </c>
       <c r="R91" t="n">
-        <v>80500</v>
+        <v>112000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>